<commit_message>
Made collection_group_id unique for EOS/EOT/Study Continuation
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_DS.xlsx
+++ b/curation/draft/collection/collection_specialization_DS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76257EDC-851E-7941-B20A-C892AF173423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128700E8-CF30-6442-97DC-F1F78F2F1E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="1080" windowWidth="29900" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_DS" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="195">
   <si>
     <t>package_date</t>
   </si>
@@ -524,6 +524,90 @@
   </si>
   <si>
     <t>derivation_description</t>
+  </si>
+  <si>
+    <t>ADVEVENT_EOT</t>
+  </si>
+  <si>
+    <t>ADVEVENT_EOS</t>
+  </si>
+  <si>
+    <t>ADVEVENT_CONT</t>
+  </si>
+  <si>
+    <t>DEAD_EOS</t>
+  </si>
+  <si>
+    <t>DEAD_EOT</t>
+  </si>
+  <si>
+    <t>DEAD_CONT</t>
+  </si>
+  <si>
+    <t>LACKEFFICACY_EOS</t>
+  </si>
+  <si>
+    <t>LACKEFFICACY_EOT</t>
+  </si>
+  <si>
+    <t>LACKEFFICACY_CONT</t>
+  </si>
+  <si>
+    <t>PHYDECISION_EOS</t>
+  </si>
+  <si>
+    <t>PHYDECISION_EOT</t>
+  </si>
+  <si>
+    <t>PHYDECISION_CONT</t>
+  </si>
+  <si>
+    <t>PROGDISEASE_EOS</t>
+  </si>
+  <si>
+    <t>PROGDISEASE_EOT</t>
+  </si>
+  <si>
+    <t>PROGDISEASE_CONT</t>
+  </si>
+  <si>
+    <t>PROTCOMP_EOS</t>
+  </si>
+  <si>
+    <t>PROTCOMP_EOT</t>
+  </si>
+  <si>
+    <t>PROTCOMP_CONT</t>
+  </si>
+  <si>
+    <t>PROTDEV_EOS</t>
+  </si>
+  <si>
+    <t>PROTDEV_EOT</t>
+  </si>
+  <si>
+    <t>PROTDEV_CONT</t>
+  </si>
+  <si>
+    <t>SUBJPREG_EOS</t>
+  </si>
+  <si>
+    <t>SUBJPREG_EOT</t>
+  </si>
+  <si>
+    <t>SUBJPREG_CONT</t>
+  </si>
+  <si>
+    <t>SUBJWITHDRAW_EOS</t>
+  </si>
+  <si>
+    <t>SUBJWITHDRAW_EOT</t>
+  </si>
+  <si>
+    <t>SUBJWITHDRAW_CONT</t>
+  </si>
+  <si>
+    <t>LTFUP_EOS</t>
   </si>
 </sst>
 </file>
@@ -929,10 +1013,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="X104" sqref="X104"/>
+      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1611,7 +1695,7 @@
         <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="J10" t="s">
         <v>127</v>
@@ -1682,7 +1766,7 @@
         <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="J11" t="s">
         <v>127</v>
@@ -1752,7 +1836,7 @@
         <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="J12" t="s">
         <v>127</v>
@@ -1821,7 +1905,7 @@
         <v>37</v>
       </c>
       <c r="H13" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="J13" t="s">
         <v>127</v>
@@ -1880,7 +1964,7 @@
         <v>37</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="J14" t="s">
         <v>127</v>
@@ -1939,7 +2023,7 @@
         <v>37</v>
       </c>
       <c r="H15" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="J15" t="s">
         <v>127</v>
@@ -2011,7 +2095,7 @@
         <v>37</v>
       </c>
       <c r="H16" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="J16" t="s">
         <v>127</v>
@@ -2080,7 +2164,7 @@
         <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="J17" t="s">
         <v>127</v>
@@ -2148,7 +2232,7 @@
         <v>37</v>
       </c>
       <c r="H18" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="J18" t="s">
         <v>127</v>
@@ -2205,7 +2289,7 @@
         <v>37</v>
       </c>
       <c r="H19" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="J19" t="s">
         <v>127</v>
@@ -2261,7 +2345,7 @@
         <v>37</v>
       </c>
       <c r="H20" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
       <c r="J20" t="s">
         <v>127</v>
@@ -2333,7 +2417,7 @@
         <v>37</v>
       </c>
       <c r="H21" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
       <c r="J21" t="s">
         <v>127</v>
@@ -2402,7 +2486,7 @@
         <v>37</v>
       </c>
       <c r="H22" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
       <c r="J22" t="s">
         <v>127</v>
@@ -2470,7 +2554,7 @@
         <v>37</v>
       </c>
       <c r="H23" t="s">
-        <v>100</v>
+        <v>173</v>
       </c>
       <c r="J23" t="s">
         <v>127</v>
@@ -2527,7 +2611,7 @@
         <v>37</v>
       </c>
       <c r="H24" t="s">
-        <v>104</v>
+        <v>194</v>
       </c>
       <c r="J24" t="s">
         <v>127</v>
@@ -2599,7 +2683,7 @@
         <v>37</v>
       </c>
       <c r="H25" t="s">
-        <v>104</v>
+        <v>194</v>
       </c>
       <c r="J25" t="s">
         <v>127</v>
@@ -2668,7 +2752,7 @@
         <v>37</v>
       </c>
       <c r="H26" t="s">
-        <v>104</v>
+        <v>194</v>
       </c>
       <c r="J26" t="s">
         <v>127</v>
@@ -2736,7 +2820,7 @@
         <v>37</v>
       </c>
       <c r="H27" t="s">
-        <v>104</v>
+        <v>194</v>
       </c>
       <c r="J27" t="s">
         <v>127</v>
@@ -2793,7 +2877,7 @@
         <v>37</v>
       </c>
       <c r="H28" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="J28" t="s">
         <v>127</v>
@@ -2865,7 +2949,7 @@
         <v>37</v>
       </c>
       <c r="H29" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="J29" t="s">
         <v>127</v>
@@ -2934,7 +3018,7 @@
         <v>37</v>
       </c>
       <c r="H30" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="J30" t="s">
         <v>127</v>
@@ -3002,7 +3086,7 @@
         <v>37</v>
       </c>
       <c r="H31" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="J31" t="s">
         <v>127</v>
@@ -3059,7 +3143,7 @@
         <v>37</v>
       </c>
       <c r="H32" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="J32" t="s">
         <v>127</v>
@@ -3131,7 +3215,7 @@
         <v>37</v>
       </c>
       <c r="H33" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="J33" t="s">
         <v>127</v>
@@ -3200,7 +3284,7 @@
         <v>37</v>
       </c>
       <c r="H34" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="J34" t="s">
         <v>127</v>
@@ -3268,7 +3352,7 @@
         <v>37</v>
       </c>
       <c r="H35" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="J35" t="s">
         <v>127</v>
@@ -3325,7 +3409,7 @@
         <v>37</v>
       </c>
       <c r="H36" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="J36" t="s">
         <v>127</v>
@@ -3397,7 +3481,7 @@
         <v>37</v>
       </c>
       <c r="H37" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="J37" t="s">
         <v>127</v>
@@ -3466,7 +3550,7 @@
         <v>37</v>
       </c>
       <c r="H38" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="J38" t="s">
         <v>127</v>
@@ -3534,7 +3618,7 @@
         <v>37</v>
       </c>
       <c r="H39" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="J39" t="s">
         <v>127</v>
@@ -3591,7 +3675,7 @@
         <v>37</v>
       </c>
       <c r="H40" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="J40" t="s">
         <v>127</v>
@@ -3663,7 +3747,7 @@
         <v>37</v>
       </c>
       <c r="H41" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="J41" t="s">
         <v>127</v>
@@ -3732,7 +3816,7 @@
         <v>37</v>
       </c>
       <c r="H42" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="J42" t="s">
         <v>127</v>
@@ -3800,7 +3884,7 @@
         <v>37</v>
       </c>
       <c r="H43" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="J43" t="s">
         <v>127</v>
@@ -3857,7 +3941,7 @@
         <v>37</v>
       </c>
       <c r="H44" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="J44" t="s">
         <v>127</v>
@@ -3929,7 +4013,7 @@
         <v>37</v>
       </c>
       <c r="H45" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="J45" t="s">
         <v>127</v>
@@ -3998,7 +4082,7 @@
         <v>37</v>
       </c>
       <c r="H46" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="J46" t="s">
         <v>127</v>
@@ -4066,7 +4150,7 @@
         <v>37</v>
       </c>
       <c r="H47" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
       <c r="J47" t="s">
         <v>127</v>
@@ -4123,7 +4207,7 @@
         <v>37</v>
       </c>
       <c r="H48" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="J48" t="s">
         <v>127</v>
@@ -4195,7 +4279,7 @@
         <v>37</v>
       </c>
       <c r="H49" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="J49" t="s">
         <v>127</v>
@@ -4264,7 +4348,7 @@
         <v>37</v>
       </c>
       <c r="H50" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="J50" t="s">
         <v>127</v>
@@ -4332,7 +4416,7 @@
         <v>37</v>
       </c>
       <c r="H51" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="J51" t="s">
         <v>127</v>
@@ -4389,7 +4473,7 @@
         <v>37</v>
       </c>
       <c r="H52" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="J52" t="s">
         <v>131</v>
@@ -4460,7 +4544,7 @@
         <v>37</v>
       </c>
       <c r="H53" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="J53" t="s">
         <v>131</v>
@@ -4528,7 +4612,7 @@
         <v>37</v>
       </c>
       <c r="H54" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="J54" t="s">
         <v>131</v>
@@ -4599,7 +4683,7 @@
         <v>37</v>
       </c>
       <c r="H55" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="J55" t="s">
         <v>131</v>
@@ -4655,7 +4739,7 @@
         <v>37</v>
       </c>
       <c r="H56" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="J56" t="s">
         <v>131</v>
@@ -4711,7 +4795,7 @@
         <v>37</v>
       </c>
       <c r="H57" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="J57" t="s">
         <v>131</v>
@@ -4783,7 +4867,7 @@
         <v>37</v>
       </c>
       <c r="H58" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="J58" t="s">
         <v>131</v>
@@ -4852,7 +4936,7 @@
         <v>37</v>
       </c>
       <c r="H59" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="J59" t="s">
         <v>131</v>
@@ -4920,7 +5004,7 @@
         <v>37</v>
       </c>
       <c r="H60" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="J60" t="s">
         <v>131</v>
@@ -4977,7 +5061,7 @@
         <v>37</v>
       </c>
       <c r="H61" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="J61" t="s">
         <v>131</v>
@@ -5034,7 +5118,7 @@
         <v>37</v>
       </c>
       <c r="H62" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="J62" t="s">
         <v>131</v>
@@ -5106,7 +5190,7 @@
         <v>37</v>
       </c>
       <c r="H63" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="J63" t="s">
         <v>131</v>
@@ -5175,7 +5259,7 @@
         <v>37</v>
       </c>
       <c r="H64" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="J64" t="s">
         <v>131</v>
@@ -5243,7 +5327,7 @@
         <v>37</v>
       </c>
       <c r="H65" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="J65" t="s">
         <v>131</v>
@@ -5300,7 +5384,7 @@
         <v>37</v>
       </c>
       <c r="H66" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="J66" t="s">
         <v>131</v>
@@ -5372,7 +5456,7 @@
         <v>37</v>
       </c>
       <c r="H67" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="J67" t="s">
         <v>131</v>
@@ -5441,7 +5525,7 @@
         <v>37</v>
       </c>
       <c r="H68" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="J68" t="s">
         <v>131</v>
@@ -5509,7 +5593,7 @@
         <v>37</v>
       </c>
       <c r="H69" t="s">
-        <v>108</v>
+        <v>177</v>
       </c>
       <c r="J69" t="s">
         <v>131</v>
@@ -5566,7 +5650,7 @@
         <v>37</v>
       </c>
       <c r="H70" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="J70" t="s">
         <v>131</v>
@@ -5638,7 +5722,7 @@
         <v>37</v>
       </c>
       <c r="H71" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="J71" t="s">
         <v>131</v>
@@ -5707,7 +5791,7 @@
         <v>37</v>
       </c>
       <c r="H72" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="J72" t="s">
         <v>131</v>
@@ -5775,7 +5859,7 @@
         <v>37</v>
       </c>
       <c r="H73" t="s">
-        <v>112</v>
+        <v>180</v>
       </c>
       <c r="J73" t="s">
         <v>131</v>
@@ -5832,7 +5916,7 @@
         <v>37</v>
       </c>
       <c r="H74" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="J74" t="s">
         <v>131</v>
@@ -5904,7 +5988,7 @@
         <v>37</v>
       </c>
       <c r="H75" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="J75" t="s">
         <v>131</v>
@@ -5973,7 +6057,7 @@
         <v>37</v>
       </c>
       <c r="H76" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="J76" t="s">
         <v>131</v>
@@ -6041,7 +6125,7 @@
         <v>37</v>
       </c>
       <c r="H77" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="J77" t="s">
         <v>131</v>
@@ -6098,7 +6182,7 @@
         <v>37</v>
       </c>
       <c r="H78" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="J78" t="s">
         <v>131</v>
@@ -6170,7 +6254,7 @@
         <v>37</v>
       </c>
       <c r="H79" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="J79" t="s">
         <v>131</v>
@@ -6239,7 +6323,7 @@
         <v>37</v>
       </c>
       <c r="H80" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="J80" t="s">
         <v>131</v>
@@ -6307,7 +6391,7 @@
         <v>37</v>
       </c>
       <c r="H81" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="J81" t="s">
         <v>131</v>
@@ -6364,7 +6448,7 @@
         <v>37</v>
       </c>
       <c r="H82" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="J82" t="s">
         <v>131</v>
@@ -6436,7 +6520,7 @@
         <v>37</v>
       </c>
       <c r="H83" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="J83" t="s">
         <v>131</v>
@@ -6505,7 +6589,7 @@
         <v>37</v>
       </c>
       <c r="H84" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="J84" t="s">
         <v>131</v>
@@ -6573,7 +6657,7 @@
         <v>37</v>
       </c>
       <c r="H85" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="J85" t="s">
         <v>131</v>
@@ -6630,7 +6714,7 @@
         <v>37</v>
       </c>
       <c r="H86" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="J86" t="s">
         <v>131</v>
@@ -6702,7 +6786,7 @@
         <v>37</v>
       </c>
       <c r="H87" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="J87" t="s">
         <v>131</v>
@@ -6771,7 +6855,7 @@
         <v>37</v>
       </c>
       <c r="H88" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="J88" t="s">
         <v>131</v>
@@ -6839,7 +6923,7 @@
         <v>37</v>
       </c>
       <c r="H89" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="J89" t="s">
         <v>131</v>
@@ -7950,7 +8034,7 @@
         <v>37</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="J106" t="s">
         <v>145</v>
@@ -8021,7 +8105,7 @@
         <v>37</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="J107" t="s">
         <v>145</v>
@@ -8089,7 +8173,7 @@
         <v>37</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="J108" t="s">
         <v>145</v>
@@ -8159,7 +8243,7 @@
         <v>37</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="J109" t="s">
         <v>145</v>
@@ -8218,7 +8302,7 @@
         <v>37</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="J110" t="s">
         <v>145</v>
@@ -8278,7 +8362,7 @@
         <v>37</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="J111" t="s">
         <v>145</v>
@@ -8350,7 +8434,7 @@
         <v>37</v>
       </c>
       <c r="H112" s="5" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="J112" t="s">
         <v>145</v>
@@ -8419,7 +8503,7 @@
         <v>37</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="J113" t="s">
         <v>145</v>
@@ -8487,7 +8571,7 @@
         <v>37</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="J114" t="s">
         <v>145</v>
@@ -8544,7 +8628,7 @@
         <v>37</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="J115" t="s">
         <v>145</v>
@@ -9129,7 +9213,7 @@
         <v>37</v>
       </c>
       <c r="H124" t="s">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J124" t="s">
         <v>145</v>
@@ -9201,7 +9285,7 @@
         <v>37</v>
       </c>
       <c r="H125" t="s">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J125" t="s">
         <v>145</v>
@@ -9268,7 +9352,7 @@
         <v>37</v>
       </c>
       <c r="H126" t="s">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J126" t="s">
         <v>145</v>
@@ -9336,7 +9420,7 @@
         <v>37</v>
       </c>
       <c r="H127" t="s">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="J127" t="s">
         <v>145</v>
@@ -9393,7 +9477,7 @@
         <v>37</v>
       </c>
       <c r="H128" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="J128" t="s">
         <v>145</v>
@@ -9465,7 +9549,7 @@
         <v>37</v>
       </c>
       <c r="H129" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="J129" t="s">
         <v>145</v>
@@ -9532,7 +9616,7 @@
         <v>37</v>
       </c>
       <c r="H130" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="J130" t="s">
         <v>145</v>
@@ -9600,7 +9684,7 @@
         <v>37</v>
       </c>
       <c r="H131" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="J131" t="s">
         <v>145</v>
@@ -9657,7 +9741,7 @@
         <v>37</v>
       </c>
       <c r="H132" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="J132" t="s">
         <v>145</v>
@@ -9729,7 +9813,7 @@
         <v>37</v>
       </c>
       <c r="H133" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="J133" t="s">
         <v>145</v>
@@ -9796,7 +9880,7 @@
         <v>37</v>
       </c>
       <c r="H134" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="J134" t="s">
         <v>145</v>
@@ -9864,7 +9948,7 @@
         <v>37</v>
       </c>
       <c r="H135" t="s">
-        <v>112</v>
+        <v>181</v>
       </c>
       <c r="J135" t="s">
         <v>145</v>
@@ -9921,7 +10005,7 @@
         <v>37</v>
       </c>
       <c r="H136" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="J136" t="s">
         <v>145</v>
@@ -9993,7 +10077,7 @@
         <v>37</v>
       </c>
       <c r="H137" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="J137" t="s">
         <v>145</v>
@@ -10060,7 +10144,7 @@
         <v>37</v>
       </c>
       <c r="H138" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="J138" t="s">
         <v>145</v>
@@ -10128,7 +10212,7 @@
         <v>37</v>
       </c>
       <c r="H139" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="J139" t="s">
         <v>145</v>
@@ -10185,7 +10269,7 @@
         <v>37</v>
       </c>
       <c r="H140" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="J140" t="s">
         <v>145</v>
@@ -10257,7 +10341,7 @@
         <v>37</v>
       </c>
       <c r="H141" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="J141" t="s">
         <v>145</v>
@@ -10324,7 +10408,7 @@
         <v>37</v>
       </c>
       <c r="H142" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="J142" t="s">
         <v>145</v>
@@ -10392,7 +10476,7 @@
         <v>37</v>
       </c>
       <c r="H143" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="J143" t="s">
         <v>145</v>
@@ -10449,7 +10533,7 @@
         <v>37</v>
       </c>
       <c r="H144" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="J144" t="s">
         <v>145</v>
@@ -10521,7 +10605,7 @@
         <v>37</v>
       </c>
       <c r="H145" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="J145" t="s">
         <v>145</v>
@@ -10588,7 +10672,7 @@
         <v>37</v>
       </c>
       <c r="H146" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="J146" t="s">
         <v>145</v>
@@ -10656,7 +10740,7 @@
         <v>37</v>
       </c>
       <c r="H147" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="J147" t="s">
         <v>145</v>
@@ -10713,7 +10797,7 @@
         <v>37</v>
       </c>
       <c r="H148" t="s">
-        <v>124</v>
+        <v>193</v>
       </c>
       <c r="J148" t="s">
         <v>145</v>
@@ -10785,7 +10869,7 @@
         <v>37</v>
       </c>
       <c r="H149" t="s">
-        <v>124</v>
+        <v>193</v>
       </c>
       <c r="J149" t="s">
         <v>145</v>
@@ -10852,7 +10936,7 @@
         <v>37</v>
       </c>
       <c r="H150" t="s">
-        <v>124</v>
+        <v>193</v>
       </c>
       <c r="J150" t="s">
         <v>145</v>
@@ -10920,7 +11004,7 @@
         <v>37</v>
       </c>
       <c r="H151" t="s">
-        <v>124</v>
+        <v>193</v>
       </c>
       <c r="J151" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
Fixed CODELIST_TERM_CCODE_MISMATCH for CONSWDRL
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_DS.xlsx
+++ b/curation/draft/collection/collection_specialization_DS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B357049-D489-4433-8AED-37DCE9FF9073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE6173E-9285-6D45-8F9D-BA15FAD43A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="915" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="2000" windowWidth="29900" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_DS" sheetId="1" r:id="rId1"/>
@@ -1017,30 +1017,30 @@
   <dimension ref="A1:AJ155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="H93" sqref="H93"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="30.33203125" customWidth="1"/>
     <col min="12" max="12" width="29" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="46.140625" customWidth="1"/>
-    <col min="17" max="17" width="31.140625" customWidth="1"/>
-    <col min="27" max="27" width="20.42578125" customWidth="1"/>
-    <col min="28" max="28" width="42.140625" style="4" customWidth="1"/>
-    <col min="29" max="29" width="22.28515625" style="4" customWidth="1"/>
-    <col min="30" max="30" width="13.85546875" customWidth="1"/>
-    <col min="31" max="31" width="36.42578125" customWidth="1"/>
-    <col min="32" max="32" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="16" max="16" width="46.1640625" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
+    <col min="27" max="27" width="20.5" customWidth="1"/>
+    <col min="28" max="28" width="42.1640625" style="4" customWidth="1"/>
+    <col min="29" max="29" width="22.33203125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="13.83203125" customWidth="1"/>
+    <col min="31" max="31" width="36.5" customWidth="1"/>
+    <col min="32" max="32" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>123</v>
       </c>
@@ -1213,8 +1213,8 @@
       <c r="AE2" t="s">
         <v>74</v>
       </c>
-      <c r="AF2" t="s">
-        <v>84</v>
+      <c r="AF2" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="AG2" t="s">
         <v>39</v>
@@ -1223,7 +1223,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>123</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>123</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>123</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>66</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>66</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>66</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>66</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>80</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>80</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>80</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>80</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>80</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>95</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>95</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>95</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>95</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>95</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>99</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>99</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>99</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>99</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>103</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>103</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>103</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>103</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>107</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>107</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>107</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>107</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>111</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>111</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>111</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>111</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>115</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>115</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>115</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>115</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>123</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>123</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>123</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>123</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>119</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>119</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>119</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>119</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>123</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>123</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>123</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>123</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>80</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>80</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>80</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>80</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>80</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>95</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>95</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>95</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>95</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>95</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>99</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>99</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>99</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>99</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>107</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>107</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>107</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>107</v>
       </c>
@@ -5636,7 +5636,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>111</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>111</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>111</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="73" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>111</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>115</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>115</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>115</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>115</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>123</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>123</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>123</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>123</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>119</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>119</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>119</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>119</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>123</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>123</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>123</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="89" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>123</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>33</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>33</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>33</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="93" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>33</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>33</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>33</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>33</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="97" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>33</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="98" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>60</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="99" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>60</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>60</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="101" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>60</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="102" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>71</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>71</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>71</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>71</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="106" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>80</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="107" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>80</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>80</v>
       </c>
@@ -8229,7 +8229,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="109" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>80</v>
       </c>
@@ -8288,7 +8288,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="110" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>80</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="111" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>95</v>
       </c>
@@ -8420,7 +8420,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>95</v>
       </c>
@@ -8489,7 +8489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>95</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="114" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>95</v>
       </c>
@@ -8614,7 +8614,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="115" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>95</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>123</v>
       </c>
@@ -8743,7 +8743,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>123</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>123</v>
       </c>
@@ -8879,7 +8879,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>123</v>
       </c>
@@ -8937,7 +8937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="120" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>123</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>123</v>
       </c>
@@ -9073,7 +9073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>123</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="123" spans="2:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>123</v>
       </c>
@@ -9199,7 +9199,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="124" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>99</v>
       </c>
@@ -9271,7 +9271,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="125" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>99</v>
       </c>
@@ -9338,7 +9338,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="126" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>99</v>
       </c>
@@ -9406,7 +9406,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>99</v>
       </c>
@@ -9463,7 +9463,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="128" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>107</v>
       </c>
@@ -9535,7 +9535,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>107</v>
       </c>
@@ -9602,7 +9602,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="130" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>107</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="131" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>107</v>
       </c>
@@ -9727,7 +9727,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="132" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>111</v>
       </c>
@@ -9799,7 +9799,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>111</v>
       </c>
@@ -9866,7 +9866,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="134" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>111</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="135" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>111</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>115</v>
       </c>
@@ -10063,7 +10063,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="137" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>115</v>
       </c>
@@ -10130,7 +10130,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>115</v>
       </c>
@@ -10198,7 +10198,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="139" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>115</v>
       </c>
@@ -10255,7 +10255,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="140" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>123</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="141" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>123</v>
       </c>
@@ -10394,7 +10394,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="142" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>123</v>
       </c>
@@ -10462,7 +10462,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="143" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>123</v>
       </c>
@@ -10519,7 +10519,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="144" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>119</v>
       </c>
@@ -10591,7 +10591,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="145" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>119</v>
       </c>
@@ -10658,7 +10658,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="146" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>119</v>
       </c>
@@ -10726,7 +10726,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>119</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>123</v>
       </c>
@@ -10855,7 +10855,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="149" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>123</v>
       </c>
@@ -10922,7 +10922,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="150" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>123</v>
       </c>
@@ -10990,7 +10990,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="151" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>123</v>
       </c>
@@ -11047,7 +11047,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="152" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>71</v>
       </c>
@@ -11120,7 +11120,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="153" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>71</v>
       </c>
@@ -11181,7 +11181,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="154" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>71</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="155" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>71</v>
       </c>

</xml_diff>